<commit_message>
new results abou BSD without turns
</commit_message>
<xml_diff>
--- a/results_BSD_withT_10_10.xlsx
+++ b/results_BSD_withT_10_10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhoumengjie/Desktop/route-finder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB7C9CB-AE94-6E41-B952-54CA2C7D3C90}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CFA578-2DBA-5D40-85BE-748BBD70BE9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="460" windowWidth="25440" windowHeight="14400" xr2:uid="{DCF972A8-F625-F14C-9F98-97D2BB9C3957}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="25440" windowHeight="14400" xr2:uid="{DCF972A8-F625-F14C-9F98-97D2BB9C3957}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="12">
   <si>
     <t>edinburgh</t>
   </si>
@@ -445,19 +445,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8D9F61-A412-744D-8F23-E4AC4AB96654}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="10" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="16.1640625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -485,8 +487,35 @@
       <c r="I1" s="2">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2">
+        <v>5</v>
+      </c>
+      <c r="M1" s="2">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2">
+        <v>15</v>
+      </c>
+      <c r="O1" s="2">
+        <v>20</v>
+      </c>
+      <c r="P1" s="2">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>30</v>
+      </c>
+      <c r="R1" s="2">
+        <v>35</v>
+      </c>
+      <c r="S1" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -514,8 +543,35 @@
       <c r="I2" s="1">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.214</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0.43</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="P2" s="1">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0.90600000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -543,8 +599,35 @@
       <c r="I3" s="1">
         <v>0.99399999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0.92800000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -572,8 +655,11 @@
       <c r="I4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K4" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -601,8 +687,11 @@
       <c r="I5" s="1">
         <v>0.96599999999999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -630,8 +719,11 @@
       <c r="I6" s="1">
         <v>0.96199999999999997</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K6" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -659,8 +751,11 @@
       <c r="I7" s="1">
         <v>0.97799999999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -688,8 +783,11 @@
       <c r="I8" s="1">
         <v>0.98599999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -717,11 +815,14 @@
       <c r="I9" s="1">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
@@ -749,8 +850,35 @@
       <c r="I15" s="2">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L15" s="2">
+        <v>5</v>
+      </c>
+      <c r="M15" s="2">
+        <v>10</v>
+      </c>
+      <c r="N15" s="2">
+        <v>15</v>
+      </c>
+      <c r="O15" s="2">
+        <v>20</v>
+      </c>
+      <c r="P15" s="2">
+        <v>25</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>30</v>
+      </c>
+      <c r="R15" s="2">
+        <v>35</v>
+      </c>
+      <c r="S15" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>0</v>
       </c>
@@ -778,8 +906,35 @@
       <c r="I16" s="1">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="O16" s="1">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="P16" s="1">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0.96799999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
@@ -807,8 +962,35 @@
       <c r="I17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L17" s="1">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="M17" s="1">
+        <v>0.248</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="O17" s="1">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="P17" s="1">
+        <v>0.876</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="R17" s="1">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="S17" s="1">
+        <v>0.98399999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>2</v>
       </c>
@@ -836,8 +1018,11 @@
       <c r="I18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K18" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
@@ -865,8 +1050,11 @@
       <c r="I19" s="1">
         <v>0.996</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K19" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>4</v>
       </c>
@@ -894,8 +1082,11 @@
       <c r="I20" s="1">
         <v>0.98799999999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K20" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>5</v>
       </c>
@@ -923,8 +1114,11 @@
       <c r="I21" s="1">
         <v>0.99399999999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K21" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>6</v>
       </c>
@@ -952,8 +1146,11 @@
       <c r="I22" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K22" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>11</v>
       </c>
@@ -981,8 +1178,11 @@
       <c r="I23" s="1">
         <v>0.96199999999999997</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K23" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>9</v>
       </c>
@@ -1010,8 +1210,35 @@
       <c r="I29" s="2">
         <v>40</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L29" s="2">
+        <v>5</v>
+      </c>
+      <c r="M29" s="2">
+        <v>10</v>
+      </c>
+      <c r="N29" s="2">
+        <v>15</v>
+      </c>
+      <c r="O29" s="2">
+        <v>20</v>
+      </c>
+      <c r="P29" s="2">
+        <v>25</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>30</v>
+      </c>
+      <c r="R29" s="2">
+        <v>35</v>
+      </c>
+      <c r="S29" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>1</v>
       </c>
@@ -1039,8 +1266,35 @@
       <c r="I30" s="1">
         <v>0.99399999999999999</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K30" s="3">
+        <v>1</v>
+      </c>
+      <c r="L30" s="1">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="M30" s="1">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="N30" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="O30" s="1">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="P30" s="1">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="R30" s="1">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="S30" s="1">
+        <v>0.92800000000000005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>5</v>
       </c>
@@ -1068,8 +1322,35 @@
       <c r="I31" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K31" s="3">
+        <v>5</v>
+      </c>
+      <c r="L31" s="1">
+        <v>0.122</v>
+      </c>
+      <c r="M31" s="1">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="N31" s="1">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="O31" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="P31" s="1">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>1</v>
+      </c>
+      <c r="R31" s="1">
+        <v>1</v>
+      </c>
+      <c r="S31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>10</v>
       </c>
@@ -1097,8 +1378,35 @@
       <c r="I32" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K32" s="3">
+        <v>10</v>
+      </c>
+      <c r="L32" s="1">
+        <v>0.214</v>
+      </c>
+      <c r="M32" s="1">
+        <v>0.502</v>
+      </c>
+      <c r="N32" s="1">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="O32" s="1">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="P32" s="1">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>1</v>
+      </c>
+      <c r="R32" s="1">
+        <v>1</v>
+      </c>
+      <c r="S32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>15</v>
       </c>
@@ -1126,8 +1434,35 @@
       <c r="I33" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K33" s="3">
+        <v>15</v>
+      </c>
+      <c r="L33" s="1">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="M33" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="N33" s="1">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="O33" s="1">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="P33" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>1</v>
+      </c>
+      <c r="R33" s="1">
+        <v>1</v>
+      </c>
+      <c r="S33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>20</v>
       </c>
@@ -1155,10 +1490,37 @@
       <c r="I34" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K34" s="3">
+        <v>20</v>
+      </c>
+      <c r="L34" s="1">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="M34" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="N34" s="1">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="O34" s="1">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="P34" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>1</v>
+      </c>
+      <c r="R34" s="1">
+        <v>1</v>
+      </c>
+      <c r="S34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>10</v>
       </c>
@@ -1186,8 +1548,35 @@
       <c r="I40" s="2">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K40" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L40" s="2">
+        <v>5</v>
+      </c>
+      <c r="M40" s="2">
+        <v>10</v>
+      </c>
+      <c r="N40" s="2">
+        <v>15</v>
+      </c>
+      <c r="O40" s="2">
+        <v>20</v>
+      </c>
+      <c r="P40" s="2">
+        <v>25</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>30</v>
+      </c>
+      <c r="R40" s="2">
+        <v>35</v>
+      </c>
+      <c r="S40" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>100</v>
       </c>
@@ -1215,8 +1604,35 @@
       <c r="I41" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K41" s="3">
+        <v>100</v>
+      </c>
+      <c r="L41" s="1">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="M41" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="N41" s="1">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="O41" s="1">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="P41" s="1">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="Q41" s="1">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="R41" s="1">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="S41" s="1">
+        <v>0.98599999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>200</v>
       </c>
@@ -1244,8 +1660,35 @@
       <c r="I42" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K42" s="3">
+        <v>200</v>
+      </c>
+      <c r="L42" s="1">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="M42" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="N42" s="1">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="O42" s="1">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="P42" s="1">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="Q42" s="1">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="R42" s="1">
+        <v>0.996</v>
+      </c>
+      <c r="S42" s="1">
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>300</v>
       </c>
@@ -1273,8 +1716,35 @@
       <c r="I43" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K43" s="3">
+        <v>300</v>
+      </c>
+      <c r="L43" s="1">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="M43" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="N43" s="1">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="O43" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="P43" s="1">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="R43" s="1">
+        <v>1</v>
+      </c>
+      <c r="S43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>400</v>
       </c>
@@ -1302,8 +1772,35 @@
       <c r="I44" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K44" s="3">
+        <v>400</v>
+      </c>
+      <c r="L44" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="M44" s="1">
+        <v>0.41</v>
+      </c>
+      <c r="N44" s="1">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="O44" s="1">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="P44" s="1">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="R44" s="1">
+        <v>1</v>
+      </c>
+      <c r="S44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>500</v>
       </c>
@@ -1329,6 +1826,33 @@
         <v>1</v>
       </c>
       <c r="I45" s="1">
+        <v>1</v>
+      </c>
+      <c r="K45" s="3">
+        <v>500</v>
+      </c>
+      <c r="L45" s="1">
+        <v>0.218</v>
+      </c>
+      <c r="M45" s="1">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="N45" s="1">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="O45" s="1">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="P45" s="1">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="R45" s="1">
+        <v>1</v>
+      </c>
+      <c r="S45" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>